<commit_message>
includes pre Start/End Times
</commit_message>
<xml_diff>
--- a/extractor/16DaySept.xlsx
+++ b/extractor/16DaySept.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/51a3ec21316aeaae/Documents/python/16day/extractor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F368A852-417C-498F-9015-FE0B04BC6BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89265B71-6F67-4E79-9492-FAABDAB834BB}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F368A852-417C-498F-9015-FE0B04BC6BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E26FF1F-6F58-490F-94C1-A5948ACE9294}"/>
   <bookViews>
-    <workbookView xWindow="15960" yWindow="0" windowWidth="9730" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report1694179558854" sheetId="1" r:id="rId1"/>
@@ -1103,10 +1103,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1406,7 +1402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H339"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="G254" sqref="G254"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7804,7 +7802,7 @@
         <v>20</v>
       </c>
       <c r="G253" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H253" s="4">
         <v>45201</v>

</xml_diff>